<commit_message>
Upgrade test files to Excel 2016.
</commit_message>
<xml_diff>
--- a/OpenXmlImports.Tests/TestFiles/Duplicated_Columns.xlsx
+++ b/OpenXmlImports.Tests/TestFiles/Duplicated_Columns.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\git\openxmlimports\OpenXmlImports.Tests\TestFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="24" windowWidth="15300" windowHeight="9528"/>
+    <workbookView xWindow="0" yWindow="20" windowWidth="15300" windowHeight="9530"/>
   </bookViews>
   <sheets>
     <sheet name="Item 1s" sheetId="1" r:id="rId1"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -76,6 +81,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -124,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -159,7 +167,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,16 +378,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -407,7 +413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>654</v>
       </c>
@@ -418,7 +424,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>655</v>
       </c>

</xml_diff>

<commit_message>
Update dependencies and update test files to Office 2016.
</commit_message>
<xml_diff>
--- a/OpenXmlImports.Tests/TestFiles/Duplicated_Columns.xlsx
+++ b/OpenXmlImports.Tests/TestFiles/Duplicated_Columns.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="20" windowWidth="15300" windowHeight="9530"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="15300" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Item 1s" sheetId="1" r:id="rId1"/>
@@ -378,14 +378,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,7 +401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -413,7 +415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>654</v>
       </c>
@@ -424,7 +426,7 @@
         <v>41275</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>655</v>
       </c>

</xml_diff>